<commit_message>
Modifies sinatra test case
</commit_message>
<xml_diff>
--- a/test cases/add_song_sinatra.xlsx
+++ b/test cases/add_song_sinatra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarPapa\repo\final-project\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A277D21-9C62-4F58-BFBE-5A443306E114}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592B8C77-E983-4D17-B1EB-8FA346567F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -203,580 +203,61 @@
 logoutLink:</t>
   </si>
   <si>
-    <t>Hacer Login en Songs by sinatra</t>
-  </si>
-  <si>
-    <t>Tener usuario y contraseña validos, y browser chrome instalado.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elementos pagina inicio:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>pageTitle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>linkText -&gt; "Songs By Sinatra"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>linksMenu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> xpath = //ul</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>sinatraImg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>xpath = //img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>loginLink</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> linkText-&gt; "log in ", xpath -&gt; "//a[contains(@href,'login')]"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elementos pagina inicio: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>loginLink</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> linkText-&gt; "log in ", xpath -&gt; "//a[contains(@href,'login')]"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Elementos pagina de login:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>userField</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> id="username"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>passField</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>id="password"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>loginButton</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>xpath = "//input[@value = 'Log In'  ]"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Elementos de pagina de inicio despues de login:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>pageTitle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:   </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>linkText -&gt; "Songs By Sinatra"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>linksMenu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>xpath = //ul</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>sinatraImg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> xpath = //img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>logoutLink</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:  </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">linkText-&gt; "log out ", xpath -&gt; "//a[contains(@href,'logout')]"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>welcomeLabel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> xpath--&gt; "//div[text()="You are now logged in as frank"]"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+    <t>Busuqeda y Filtro en Amazón</t>
+  </si>
+  <si>
+    <t>browser chrome instalado.</t>
+  </si>
+  <si>
+    <t>Navegar a la URL de Amazón Mexico</t>
+  </si>
+  <si>
+    <t>Se carga la página correctamente</t>
+  </si>
+  <si>
+    <t>Buscar articulo</t>
+  </si>
+  <si>
+    <t>Se visualiza un listado de productos</t>
+  </si>
+  <si>
+    <t>Filtrar por marca el producto</t>
+  </si>
+  <si>
+    <t>Se visualizan productos de la marca filtrada</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.mx/ref=nav_logo</t>
+  </si>
+  <si>
+    <t>Guantes de boxeo</t>
+  </si>
+  <si>
+    <t>Everlast</t>
+  </si>
+  <si>
+    <t>Title: Título de la página
+Campo de búsqueda
+Botón de bpusqueda
+Search results page:
+listado de marcas
+listado de articulos.</t>
+  </si>
+  <si>
+    <t>listado de las marcas
+Listado de los artículos filtrados</t>
+  </si>
+  <si>
+    <t>Title: Título de la página -&gt; "Amazon.com.mx: Precios bajos - Envío rápido - Millones de productos"
+Campo de búsqueda -&gt; id = "twotabsearchtextbox"
+Botón de bpusqueda -&gt; class="nav-input"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -798,14 +279,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -814,9 +288,8 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -849,10 +322,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -875,8 +349,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1191,22 +670,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FC4D5C-4DE3-4E3A-8BF4-1F63FC108E20}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="3" width="31.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="67.88671875" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.6640625" customWidth="1"/>
+    <col min="8" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1245,53 +724,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="115.8" customHeight="1">
+    <row r="7" spans="1:6" ht="60">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="244.8" customHeight="1">
+    <row r="8" spans="1:6" ht="105">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="14.4">
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -1301,7 +788,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1309,7 +796,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="14.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1320,8 +807,11 @@
       <c r="F12" s="9"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{0F193DFE-58C3-4264-A69F-5B8CBC0ADB64}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1329,23 +819,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E53062-28D7-4895-A4C5-0E934E6B8F13}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="42" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.6640625" customWidth="1"/>
+    <col min="8" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1384,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72">
+    <row r="7" spans="1:6" ht="75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1402,7 +892,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="216">
+    <row r="8" spans="1:6" ht="255">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1420,7 +910,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="403.2">
+    <row r="9" spans="1:6" ht="409.5">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1448,7 +938,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1458,7 +948,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="14.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1466,7 +956,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="14.4">
+    <row r="13" spans="1:6">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -1490,19 +980,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="42" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.6640625" customWidth="1"/>
+    <col min="8" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.4">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="72">
+    <row r="7" spans="1:5" ht="75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1558,7 +1048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="129.6">
+    <row r="8" spans="1:5" ht="135">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1575,7 +1065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="100.8">
+    <row r="9" spans="1:5" ht="105">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1606,7 +1096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.4">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1614,12 +1104,12 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="14.4">
+    <row r="12" spans="1:5">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="14.4">
+    <row r="13" spans="1:5">
       <c r="A13" s="4">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Removes static keyword from Hooks class members
</commit_message>
<xml_diff>
--- a/test cases/add_song_sinatra.xlsx
+++ b/test cases/add_song_sinatra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarPapa\repo\final-project\test cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\final-project\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592B8C77-E983-4D17-B1EB-8FA346567F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5211D4DC-A50B-482E-A926-0935046FCE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="3" r:id="rId1"/>
@@ -674,18 +674,18 @@
       <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="3" width="31.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="3" width="31.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="67.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.7109375" customWidth="1"/>
+    <col min="8" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -724,7 +724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
+    <row r="7" spans="1:6" ht="57.6">
       <c r="A7">
         <v>1</v>
       </c>
@@ -742,7 +742,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="105">
+    <row r="8" spans="1:6" ht="100.8">
       <c r="A8">
         <v>2</v>
       </c>
@@ -760,7 +760,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:6" ht="28.8">
       <c r="A9">
         <v>4</v>
       </c>
@@ -778,7 +778,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="14.4">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -796,7 +796,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.4">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -819,23 +819,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E53062-28D7-4895-A4C5-0E934E6B8F13}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="42" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.7109375" customWidth="1"/>
+    <col min="8" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -874,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75">
+    <row r="7" spans="1:6" ht="72">
       <c r="A7">
         <v>1</v>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="255">
+    <row r="8" spans="1:6" ht="216">
       <c r="A8">
         <v>2</v>
       </c>
@@ -910,7 +910,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="409.5">
+    <row r="9" spans="1:6" ht="403.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -948,7 +948,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.4">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -956,7 +956,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="14.4">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -980,19 +980,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="42" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.7109375" customWidth="1"/>
+    <col min="8" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="14.4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75">
+    <row r="7" spans="1:5" ht="72">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="135">
+    <row r="8" spans="1:5" ht="129.6">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="105">
+    <row r="9" spans="1:5" ht="100.8">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="14.4">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1104,12 +1104,12 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="14.4">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="14.4">
       <c r="A13" s="4">
         <v>6</v>
       </c>

</xml_diff>